<commit_message>
Sprint Backlog + some small changes...
Signed-off-by: muellers <stefan.mueller@vol.at>
</commit_message>
<xml_diff>
--- a/sprint backlog/SprintBacklog.xlsx
+++ b/sprint backlog/SprintBacklog.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT 1" sheetId="1" r:id="rId1"/>
-    <sheet name="SPRINT 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="SPRINT 2" sheetId="4" r:id="rId2"/>
+    <sheet name="SPRINT 3" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -49,8 +50,76 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>stefan</author>
+  </authors>
+  <commentList>
+    <comment ref="M10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Do not fill this column</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>stefan</author>
+  </authors>
+  <commentList>
+    <comment ref="M10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Do not fill this column</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>Task Nr.</t>
   </si>
@@ -211,7 +280,43 @@
     <t>Projekt BlueHotel - Sprintbacklog</t>
   </si>
   <si>
-    <t>to do</t>
+    <t>Reservierung mehrerer Zimmer</t>
+  </si>
+  <si>
+    <t>Überarbeitung GUI</t>
+  </si>
+  <si>
+    <t>Überarbeitung Hauptmenü</t>
+  </si>
+  <si>
+    <t>Überarbeitung Kunde GUI</t>
+  </si>
+  <si>
+    <t>Überarbeitung Zimmer GUI</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>Überarbeitung Reservierung GUI</t>
+  </si>
+  <si>
+    <t>Datenbank erweitern (neue Tabelle)</t>
+  </si>
+  <si>
+    <t>Programmierung</t>
+  </si>
+  <si>
+    <t>Rechnungen erstellen</t>
+  </si>
+  <si>
+    <t>GUI erweitern</t>
+  </si>
+  <si>
+    <t>Reservierung stornieren</t>
+  </si>
+  <si>
+    <t>Frühzeitige Abreise erfassen</t>
   </si>
 </sst>
 </file>
@@ -502,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -608,11 +713,127 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF6F7B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF6F7B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF6F7B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -780,11 +1001,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64084224"/>
-        <c:axId val="82064128"/>
+        <c:axId val="77719808"/>
+        <c:axId val="85611264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64084224"/>
+        <c:axId val="77719808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,14 +1030,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82064128"/>
+        <c:crossAx val="85611264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82064128"/>
+        <c:axId val="85611264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +1064,7 @@
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64084224"/>
+        <c:crossAx val="77719808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -856,7 +1077,405 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1400"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SPRINT 2'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idealisiert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPRINT 2'!$F$22:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5714285714285712</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7142857142857135</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2857142857142847</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8571428571428559</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4285714285714273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SPRINT 2'!$E$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Faktisch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPRINT 2'!$F$23:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="32946432"/>
+        <c:axId val="32956800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="32946432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Tage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32956800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32956800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Stunden</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32946432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1400"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SPRINT 3'!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idealisiert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPRINT 3'!$F$22:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.571428571428573</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8571428571428585</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1428571428571441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4285714285714297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7142857142857155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SPRINT 3'!$E$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Faktisch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPRINT 3'!$F$23:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="76964992"/>
+        <c:axId val="77866880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="76964992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Tage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77866880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77866880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Stunden</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76964992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -875,6 +1494,76 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
       <xdr:row>50</xdr:row>
+      <xdr:rowOff>145675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>11204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>145675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>11204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>145675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1184,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,7 +1887,7 @@
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="2.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21">
@@ -1488,7 +2177,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="24">
@@ -1516,7 +2205,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="24">
@@ -1596,7 +2285,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="24">
@@ -1632,7 +2321,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="24">
@@ -1659,7 +2348,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="24">
@@ -1705,7 +2394,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="24">
@@ -1736,7 +2425,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="24">
@@ -1763,7 +2452,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="24"/>
@@ -1805,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="24">
@@ -1838,7 +2527,7 @@
         <v>11</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="24"/>
@@ -1863,7 +2552,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="28">
@@ -1969,18 +2658,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D12:D15 D17:D19 D21:D23 D25:D27">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>$Z$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>$Z$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>$Z$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C15 C17:C19 C21:C23 C25:C27">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>$Z$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2001,25 +2690,1191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="10" customWidth="1"/>
+    <col min="26" max="26" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="21">
+      <c r="A1" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="44">
+        <v>40865</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="44">
+        <v>40871</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>3</v>
+      </c>
+      <c r="I7" s="17">
+        <v>4</v>
+      </c>
+      <c r="J7" s="17">
+        <v>5</v>
+      </c>
+      <c r="K7" s="17">
+        <v>6</v>
+      </c>
+      <c r="L7" s="18">
+        <v>7</v>
+      </c>
+      <c r="M7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="45">
+        <f>B4</f>
+        <v>40865</v>
+      </c>
+      <c r="G8" s="45">
+        <v>40859</v>
+      </c>
+      <c r="H8" s="45">
+        <v>40860</v>
+      </c>
+      <c r="I8" s="45">
+        <v>40861</v>
+      </c>
+      <c r="J8" s="45">
+        <v>40862</v>
+      </c>
+      <c r="K8" s="45">
+        <v>40863</v>
+      </c>
+      <c r="L8" s="46">
+        <v>40864</v>
+      </c>
+      <c r="M8" s="5">
+        <v>40865</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="52">
+        <f>SUM(F11:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="52">
+        <f>SUM(G11:G18)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="52">
+        <f>SUM(H11:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="52">
+        <f>SUM(I11:I18)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="52">
+        <f>SUM(J11:J18)</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="52">
+        <f>SUM(K11:K18)</f>
+        <v>2</v>
+      </c>
+      <c r="L9" s="53">
+        <f>SUM(L11:L18)</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="19">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>53</v>
       </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="35"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24">
+        <v>1</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="36"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24">
+        <v>1</v>
+      </c>
+      <c r="J13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>1</v>
+      </c>
+      <c r="M13" s="36"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="37"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24">
+        <v>2</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="36"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="36"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24">
+        <v>1</v>
+      </c>
+      <c r="L17" s="42"/>
+      <c r="M17" s="36"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="43">
+        <v>1</v>
+      </c>
+      <c r="M18" s="36"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="E21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="39"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="7"/>
+      <c r="E22" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="9">
+        <f>SUM(F9:L9)</f>
+        <v>10</v>
+      </c>
+      <c r="G22" s="10">
+        <f>F22-$F$22/7</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" ref="H22:M22" si="0">G22-$F$22/7</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857135</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142847</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8571428571428559</v>
+      </c>
+      <c r="L22" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714273</v>
+      </c>
+      <c r="M22" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="E23" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="13">
+        <f>SUM(F9:L9)</f>
+        <v>10</v>
+      </c>
+      <c r="G23" s="13">
+        <f>F23-F9</f>
+        <v>10</v>
+      </c>
+      <c r="H23" s="13">
+        <f>G23-G9</f>
+        <v>7</v>
+      </c>
+      <c r="I23" s="13">
+        <f>H23-H9</f>
+        <v>7</v>
+      </c>
+      <c r="J23" s="13">
+        <f>I23-I9</f>
+        <v>6</v>
+      </c>
+      <c r="K23" s="13">
+        <f>J23-J9</f>
+        <v>4</v>
+      </c>
+      <c r="L23" s="14">
+        <f>K23-K9</f>
+        <v>2</v>
+      </c>
+      <c r="M23" s="41">
+        <f>L23-L9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="26:26">
+      <c r="Z71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="26:26">
+      <c r="Z72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="26:26">
+      <c r="Z73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="26:26">
+      <c r="Z76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="26:26">
+      <c r="Z77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="26:26">
+      <c r="Z78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="26:26">
+      <c r="Z79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="26:26">
+      <c r="Z80" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D15:D18 D12:D13">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>$Z$73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>$Z$72</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>$Z$71</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Ungültiger Wert" sqref="D15:D18 D12:D13">
+      <formula1>$Z$71:$Z$73</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Ungültiger Wert" sqref="C12:C18">
+      <formula1>$Z$76:$Z$80</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="10" customWidth="1"/>
+    <col min="26" max="26" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21">
+      <c r="A1" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="44">
+        <v>40865</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="44">
+        <v>40871</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>3</v>
+      </c>
+      <c r="I7" s="17">
+        <v>4</v>
+      </c>
+      <c r="J7" s="17">
+        <v>5</v>
+      </c>
+      <c r="K7" s="17">
+        <v>6</v>
+      </c>
+      <c r="L7" s="18">
+        <v>7</v>
+      </c>
+      <c r="M7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="45">
+        <f>B4</f>
+        <v>40865</v>
+      </c>
+      <c r="G8" s="45">
+        <v>40859</v>
+      </c>
+      <c r="H8" s="45">
+        <v>40860</v>
+      </c>
+      <c r="I8" s="45">
+        <v>40861</v>
+      </c>
+      <c r="J8" s="45">
+        <v>40862</v>
+      </c>
+      <c r="K8" s="45">
+        <v>40863</v>
+      </c>
+      <c r="L8" s="46">
+        <v>40864</v>
+      </c>
+      <c r="M8" s="5">
+        <v>40865</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="52">
+        <f>SUM(F11:F18)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="52">
+        <f>SUM(G11:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="52">
+        <f>SUM(H11:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="52">
+        <f>SUM(I11:I18)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="52">
+        <f>SUM(J11:J18)</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="52">
+        <f>SUM(K11:K18)</f>
+        <v>3</v>
+      </c>
+      <c r="L9" s="53">
+        <f>SUM(L11:L18)</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="19">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="35"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="36"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24">
+        <v>1</v>
+      </c>
+      <c r="J13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>1</v>
+      </c>
+      <c r="M13" s="36"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24">
+        <v>1</v>
+      </c>
+      <c r="K14" s="24">
+        <v>1</v>
+      </c>
+      <c r="L14" s="42">
+        <v>1</v>
+      </c>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24">
+        <v>1</v>
+      </c>
+      <c r="L16" s="42"/>
+      <c r="M16" s="36"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="36"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28">
+        <v>1</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="36"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="E21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="39"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="7"/>
+      <c r="E22" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="9">
+        <f>SUM(F9:L9)</f>
+        <v>10</v>
+      </c>
+      <c r="G22" s="10">
+        <f>F22-$F$22/7</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" ref="H22:M22" si="0">G22-$F$22/7</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857135</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142847</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8571428571428559</v>
+      </c>
+      <c r="L22" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714273</v>
+      </c>
+      <c r="M22" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="E23" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="13">
+        <f>SUM(F9:L9)</f>
+        <v>10</v>
+      </c>
+      <c r="G23" s="13">
+        <f>F23-F9</f>
+        <v>9</v>
+      </c>
+      <c r="H23" s="13">
+        <f>G23-G9</f>
+        <v>9</v>
+      </c>
+      <c r="I23" s="13">
+        <f>H23-H9</f>
+        <v>9</v>
+      </c>
+      <c r="J23" s="13">
+        <f>I23-I9</f>
+        <v>8</v>
+      </c>
+      <c r="K23" s="13">
+        <f>J23-J9</f>
+        <v>5</v>
+      </c>
+      <c r="L23" s="14">
+        <f>K23-K9</f>
+        <v>2</v>
+      </c>
+      <c r="M23" s="41">
+        <f>L23-L9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="26:26">
+      <c r="Z71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="26:26">
+      <c r="Z72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="26:26">
+      <c r="Z73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="26:26">
+      <c r="Z76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="26:26">
+      <c r="Z77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="26:26">
+      <c r="Z78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="26:26">
+      <c r="Z79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="26:26">
+      <c r="Z80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D12:D14 D16 D18">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>$Z$73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>$Z$72</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>$Z$71</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Ungültiger Wert" sqref="C12:C18">
+      <formula1>$Z$76:$Z$80</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Ungültiger Wert" sqref="D12:D14 D18 D16">
+      <formula1>$Z$71:$Z$73</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>